<commit_message>
Inseridas os valores das correntes de core e consumo externo do processador na planilha Power Supply.xlsx.
</commit_message>
<xml_diff>
--- a/implementação/doc/Power Supply.xlsx
+++ b/implementação/doc/Power Supply.xlsx
@@ -72,29 +72,29 @@
     <t>DEVICES</t>
   </si>
   <si>
-    <t>REGULATOR</t>
-  </si>
-  <si>
-    <t>INPUT   VOLTAGE [V]</t>
-  </si>
-  <si>
-    <t>INPUT   CURRENT [mA]</t>
-  </si>
-  <si>
     <t>MAIN POWER SUPPLY</t>
   </si>
   <si>
     <t>CURRENT [A]</t>
   </si>
   <si>
-    <t>???</t>
+    <t>REGULATORS</t>
+  </si>
+  <si>
+    <t>INPUT CURRENT [mA]</t>
+  </si>
+  <si>
+    <t>INPUT VOLTAGE [V]</t>
+  </si>
+  <si>
+    <t>MAXIMUM OUTPUT CURRENT [mA]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +114,12 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -169,7 +175,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -277,11 +283,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -307,18 +333,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -373,36 +387,56 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1"/>
@@ -708,18 +742,19 @@
     <col min="1" max="1" width="7.140625" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="24.95" customHeight="1">
       <c r="B3" s="5" t="s">
@@ -728,114 +763,116 @@
       <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="29">
         <v>1.3</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="23"/>
+      <c r="D4" s="33">
+        <v>305</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A5" s="37"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="39"/>
+      <c r="B5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="C5" s="41">
+        <v>3.3</v>
+      </c>
+      <c r="D5" s="31">
         <v>1</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A6" s="37"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="33">
-        <v>3.3</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="24"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="44">
+        <v>150</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A7" s="37"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="9">
+      <c r="C7" s="42"/>
+      <c r="D7" s="27">
         <v>200</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="24"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A8" s="37"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="24"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="27">
+        <v>1</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A9" s="37"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="9">
-        <v>38</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="24"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="27">
+        <v>40</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A10" s="37"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="9">
-        <v>92</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="24"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="27">
+        <v>100</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="20"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A11" s="37"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="39"/>
+      <c r="B11" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="9">
-        <v>12.5</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="24"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="32">
+        <v>15</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A12" s="38"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
@@ -845,136 +882,134 @@
       <c r="D12" s="3">
         <v>245</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="14" spans="1:10" ht="35.1" customHeight="1">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="17" t="s">
+      <c r="D14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="21"/>
+    </row>
+    <row r="15" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A15" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="25"/>
-    </row>
-    <row r="15" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A15" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21">
+      <c r="B15" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17">
+        <v>9</v>
+      </c>
+      <c r="E15" s="17">
         <v>3.3</v>
       </c>
-      <c r="E15" s="21">
-        <v>1.3</v>
-      </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="21">
-        <f>D4</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="17">
+        <f>SUM(D5:D11)+F17</f>
+        <v>812</v>
+      </c>
+      <c r="H15" s="17">
+        <v>2000</v>
+      </c>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
     </row>
     <row r="16" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A16" s="40"/>
-      <c r="B16" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21">
-        <v>3.3</v>
-      </c>
-      <c r="E16" s="21">
-        <v>2.5</v>
-      </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="21">
-        <f>D5</f>
-        <v>1</v>
-      </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-    </row>
-    <row r="17" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A17" s="41"/>
-      <c r="B17" s="21" t="s">
+      <c r="A16" s="35"/>
+      <c r="B16" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21">
+      <c r="C16" s="10"/>
+      <c r="D16" s="10">
         <v>9</v>
       </c>
-      <c r="E17" s="21">
-        <v>3.3</v>
-      </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="21">
-        <f>SUM(D5:D11)+F15+F16</f>
-        <v>343.8</v>
-      </c>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-    </row>
-    <row r="18" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A18" s="42"/>
-      <c r="B18" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14">
-        <v>9</v>
-      </c>
-      <c r="E18" s="14">
+      <c r="E16" s="10">
         <v>5</v>
       </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="14">
+      <c r="F16" s="14"/>
+      <c r="G16" s="10">
         <f>D12</f>
         <v>245</v>
       </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
+      <c r="H16" s="10">
+        <v>1000</v>
+      </c>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A17" s="35"/>
+      <c r="B17" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17">
+        <v>3.3</v>
+      </c>
+      <c r="E17" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="F17" s="18">
+        <f>D4</f>
+        <v>305</v>
+      </c>
+      <c r="G17" s="17">
+        <f>D4</f>
+        <v>305</v>
+      </c>
+      <c r="H17" s="17">
+        <v>500</v>
+      </c>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="19" spans="1:10" ht="24.95" customHeight="1">
+      <c r="C19" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="24.95" customHeight="1">
-      <c r="C20" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="24.95" customHeight="1">
-      <c r="B21" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="30">
+      <c r="B20" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="26">
         <v>9</v>
       </c>
-      <c r="D21" s="28"/>
+      <c r="D20" s="24">
+        <f>SUM(F15:F16)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="A15:A17"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="C6:C11"/>
     <mergeCell ref="A4:A12"/>
-    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="C5:C11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>